<commit_message>
changement de mvt stock/etatsock
</commit_message>
<xml_diff>
--- a/sql/Données.xlsx
+++ b/sql/Données.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryrab\Desktop\Ryan\Etudes\S5\ArchitectureLogiciel\Matelas\matelas\Matelas\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152F1AA7-0D9E-43DC-A745-F194698EDFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17A9FD0-929E-4BB8-92E9-A3843AFB9D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{644D803D-6827-42B7-AEBC-502B0FF62A5A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
   <si>
     <t>Bloc</t>
   </si>
@@ -118,40 +118,22 @@
     <t>Prix revient</t>
   </si>
   <si>
-    <t>Nombre peut créer</t>
-  </si>
-  <si>
-    <t>Reste</t>
-  </si>
-  <si>
     <t>Somme produite</t>
   </si>
   <si>
     <t>Prix de revient</t>
   </si>
   <si>
-    <t>Prix de vente total</t>
-  </si>
-  <si>
     <t>Prix rapport volume</t>
   </si>
   <si>
     <t>RT2</t>
   </si>
   <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T6</t>
-  </si>
-  <si>
-    <t>T7</t>
-  </si>
-  <si>
-    <t>T8</t>
-  </si>
-  <si>
     <t>BR2</t>
+  </si>
+  <si>
+    <t>Prix de vente</t>
   </si>
 </sst>
 </file>
@@ -187,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -221,32 +203,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -562,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84834349-CD01-486F-9E72-82FEEE302522}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,6 +552,7 @@
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" customWidth="1"/>
     <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" customWidth="1"/>
     <col min="10" max="10" width="13.88671875" customWidth="1"/>
     <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
@@ -597,7 +574,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -627,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -635,27 +612,27 @@
         <v>5</v>
       </c>
       <c r="B2" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1000000</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3200000</v>
       </c>
       <c r="F2" s="1">
         <f>B2*C2*D2</f>
-        <v>96</v>
+        <v>420</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="1">
         <f>F2*2/100</f>
-        <v>1.92</v>
+        <v>8.4</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>10</v>
@@ -669,16 +646,16 @@
       <c r="M2" s="1">
         <v>0.5</v>
       </c>
-      <c r="N2" s="5">
-        <v>20000</v>
-      </c>
-      <c r="O2" s="9">
+      <c r="N2" s="4">
+        <v>10000</v>
+      </c>
+      <c r="O2" s="6">
         <f>K2*L2*M2</f>
         <v>1.1700000000000002</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="5">
         <f>N2/O2</f>
-        <v>17094.01709401709</v>
+        <v>8547.0085470085451</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -694,7 +671,7 @@
       <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1250000</v>
       </c>
       <c r="F3" s="1">
@@ -720,16 +697,16 @@
       <c r="M3" s="1">
         <v>0.5</v>
       </c>
-      <c r="N3" s="5">
-        <v>35000</v>
+      <c r="N3" s="4">
+        <v>25000</v>
       </c>
       <c r="O3" s="1">
         <f t="shared" ref="O3:O5" si="0">K3*L3*M3</f>
         <v>1.6500000000000001</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="5">
         <f t="shared" ref="P3:P5" si="1">N3/O3</f>
-        <v>21212.121212121212</v>
+        <v>15151.51515151515</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -737,28 +714,28 @@
         <v>20</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
         <f>F4*E2/F2</f>
-        <v>31250</v>
+        <v>1142857.142857143</v>
       </c>
       <c r="F4" s="1">
         <f>B4*C4*D4</f>
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="1">
         <f>F4*2%</f>
-        <v>0.06</v>
+        <v>3</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>12</v>
@@ -772,45 +749,45 @@
       <c r="M4" s="1">
         <v>0.75</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>32500</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="5">
         <f t="shared" si="1"/>
         <v>14444.444444444445</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>3.12</v>
       </c>
       <c r="D5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="4">
         <f>F5*E3/F3</f>
-        <v>5952.3809523809523</v>
+        <v>464285.71428571426</v>
       </c>
       <c r="F5" s="1">
         <f>B5*C5*D5</f>
-        <v>0.5</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="1">
         <f>F5*2%</f>
-        <v>0.01</v>
+        <v>0.78</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>13</v>
@@ -824,14 +801,14 @@
       <c r="M5" s="1">
         <v>0.1</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>50</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="0"/>
         <v>4.000000000000001E-3</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="5">
         <f t="shared" si="1"/>
         <v>12499.999999999996</v>
       </c>
@@ -852,8 +829,11 @@
       <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>34</v>
+      <c r="F10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>22</v>
@@ -862,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>21</v>
@@ -879,15 +859,19 @@
         <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="E11" s="1">
         <f>O2*D11</f>
-        <v>18.720000000000002</v>
-      </c>
-      <c r="F11" s="5">
+        <v>70.2</v>
+      </c>
+      <c r="F11" s="4">
+        <f>E11*$E$2/$F$2</f>
+        <v>534857.14285714284</v>
+      </c>
+      <c r="G11" s="5">
         <f>D11*N2</f>
-        <v>320000</v>
+        <v>600000</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>23</v>
@@ -897,11 +881,11 @@
       </c>
       <c r="K11" s="1">
         <f>SUM(E11:E14)</f>
-        <v>91.59</v>
-      </c>
-      <c r="L11" s="8">
+        <v>265.32</v>
+      </c>
+      <c r="L11" s="5">
         <f>F2-K11-F4</f>
-        <v>1.4099999999999966</v>
+        <v>4.6800000000000068</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -915,15 +899,33 @@
         <v>11</v>
       </c>
       <c r="D12" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1">
         <f>D12*O3</f>
-        <v>16.5</v>
-      </c>
-      <c r="F12" s="5">
-        <f t="shared" ref="F12:F14" si="2">D12*N3</f>
-        <v>350000</v>
+        <v>82.5</v>
+      </c>
+      <c r="F12" s="4">
+        <f>E12*$E$2/$F$2</f>
+        <v>628571.42857142852</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" ref="G12:G14" si="2">D12*N3</f>
+        <v>1250000</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1">
+        <f>SUM(E17:E18)</f>
+        <v>110.25</v>
+      </c>
+      <c r="L12" s="1">
+        <f>F4-K12-F5</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -937,15 +939,19 @@
         <v>12</v>
       </c>
       <c r="D13" s="1">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1">
         <f>O4*D13</f>
-        <v>56.25</v>
-      </c>
-      <c r="F13" s="5">
+        <v>112.5</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" ref="F12:F14" si="3">E13*$E$2/$F$2</f>
+        <v>857142.85714285716</v>
+      </c>
+      <c r="G13" s="5">
         <f t="shared" si="2"/>
-        <v>812500</v>
+        <v>1625000</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -965,7 +971,11 @@
         <f>O5*D14</f>
         <v>0.12000000000000002</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
+        <f t="shared" si="3"/>
+        <v>914.28571428571445</v>
+      </c>
+      <c r="G14" s="5">
         <f t="shared" si="2"/>
         <v>1500</v>
       </c>
@@ -986,294 +996,196 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="I16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="5">
-        <f>E2</f>
-        <v>1000000</v>
-      </c>
-      <c r="K16" s="5">
+      <c r="J16" s="4">
         <f>SUM(F11:F14)</f>
-        <v>1484000</v>
-      </c>
-      <c r="L16" s="5">
+        <v>2021485.7142857143</v>
+      </c>
+      <c r="K16" s="4">
+        <f>SUM(G11:G14)</f>
+        <v>3476500</v>
+      </c>
+      <c r="L16" s="4">
         <f>K16-J16</f>
-        <v>484000</v>
+        <v>1455014.2857142857</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="I17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17" s="5">
-        <f>E3</f>
-        <v>1250000</v>
-      </c>
-      <c r="K17" s="5">
-        <f>SUM(F26:F29)</f>
-        <v>1699250</v>
-      </c>
-      <c r="L17" s="5">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45</v>
+      </c>
+      <c r="E17" s="1">
+        <f>D17*O3</f>
+        <v>74.25</v>
+      </c>
+      <c r="F17" s="4">
+        <f>E17*$E$4/$F$4</f>
+        <v>565714.2857142858</v>
+      </c>
+      <c r="G17" s="5">
+        <f>D17*N3</f>
+        <v>1125000</v>
+      </c>
+      <c r="J17" s="7">
+        <f>SUM(F17:F18)</f>
+        <v>840000.00000000012</v>
+      </c>
+      <c r="K17" s="7">
+        <f>SUM(G17:G18)</f>
+        <v>1645000</v>
+      </c>
+      <c r="L17" s="7">
         <f>K17-J17</f>
-        <v>449250</v>
+        <v>804999.99999999988</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1">
+        <f>O4*D18</f>
+        <v>36</v>
+      </c>
+      <c r="F18" s="4">
+        <f>E18*$E$4/$F$4</f>
+        <v>274285.71428571432</v>
+      </c>
+      <c r="G18" s="5">
+        <f>D18*N4</f>
+        <v>520000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="10"/>
+      <c r="I19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J18" s="10">
-        <f>SUM(J16:J17)</f>
-        <v>2250000</v>
-      </c>
-      <c r="K18" s="10">
-        <f>SUM(K16:K17)</f>
-        <v>3183250</v>
-      </c>
-      <c r="L18" s="10">
-        <f>SUM(L16:L17)</f>
-        <v>933250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="6">
-        <f>INT($F$4/O2)</f>
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <f>$F$4-(INT($F$4/O2)*O2)</f>
-        <v>0.6599999999999997</v>
-      </c>
-      <c r="E19" s="7">
-        <f>P2</f>
-        <v>17094.01709401709</v>
+      <c r="L19" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="6">
-        <f t="shared" ref="C20:C22" si="3">INT($F$4/O3)</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="9">
-        <f t="shared" ref="D20:D22" si="4">$F$4-(INT($F$4/O3)*O3)</f>
-        <v>1.3499999999999999</v>
-      </c>
-      <c r="E20" s="7">
-        <f t="shared" ref="E20:E22" si="5">P3</f>
-        <v>21212.121212121212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="E21" s="7">
-        <f t="shared" si="5"/>
-        <v>14444.444444444445</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="10"/>
+      <c r="I20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="1">
+        <f>SUM(E24:E27)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>21</v>
+      <c r="L20" s="5">
+        <f>F3-K20-F5</f>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="6">
-        <f t="shared" si="3"/>
-        <v>750</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="7">
-        <f t="shared" si="5"/>
-        <v>12499.999999999996</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K22" s="1">
-        <f>SUM(E26:E29)</f>
-        <v>104.09</v>
-      </c>
-      <c r="L22" s="8">
-        <f>F3-K22-F5</f>
-        <v>0.40999999999999659</v>
-      </c>
+      <c r="F22" s="13">
+        <f>(F12+F17)/(D12+D17)</f>
+        <v>12571.428571428572</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="1">
-        <v>20</v>
-      </c>
-      <c r="E26" s="1">
-        <f>O2*D26</f>
-        <v>23.400000000000002</v>
-      </c>
-      <c r="F26" s="5">
-        <f>D26*N2</f>
-        <v>400000</v>
-      </c>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1">
-        <v>12</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" ref="E27:E29" si="6">O3*D27</f>
-        <v>19.8</v>
-      </c>
-      <c r="F27" s="5">
-        <f t="shared" ref="F27:F29" si="7">D27*N3</f>
-        <v>420000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="1">
-        <v>27</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="6"/>
-        <v>60.75</v>
-      </c>
-      <c r="F28" s="5">
-        <f t="shared" si="7"/>
-        <v>877500</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="1">
-        <v>35</v>
-      </c>
-      <c r="E29" s="1">
-        <f t="shared" si="6"/>
-        <v>0.14000000000000004</v>
-      </c>
-      <c r="F29" s="5">
-        <f t="shared" si="7"/>
-        <v>1750</v>
-      </c>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1353,7 +1265,7 @@
       <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>1000000</v>
       </c>
       <c r="F2" s="1">
@@ -1379,7 +1291,7 @@
       <c r="M2" s="1">
         <v>0.5</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="4">
         <v>20000</v>
       </c>
       <c r="O2" s="1">
@@ -1400,7 +1312,7 @@
       <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>175000</v>
       </c>
       <c r="F3" s="1">
@@ -1426,7 +1338,7 @@
       <c r="M3" s="1">
         <v>0.5</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="4">
         <v>35000</v>
       </c>
       <c r="O3" s="1">
@@ -1447,7 +1359,7 @@
       <c r="D4" s="1">
         <v>0.5</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f>B4*C4*D4</f>
         <v>3</v>
       </c>
@@ -1474,7 +1386,7 @@
       <c r="M4" s="1">
         <v>0.75</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>32500</v>
       </c>
       <c r="O4" s="1">
@@ -1495,7 +1407,7 @@
       <c r="M5" s="1">
         <v>0.1</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>200</v>
       </c>
       <c r="O5" s="1">
@@ -1552,7 +1464,7 @@
         <f>O2*D11</f>
         <v>18.720000000000002</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f>D11*N2</f>
         <v>320000</v>
       </c>
@@ -1588,7 +1500,7 @@
         <f>D12*O3</f>
         <v>16.5</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f t="shared" ref="F12:F14" si="1">D12*N3</f>
         <v>350000</v>
       </c>
@@ -1610,7 +1522,7 @@
         <f>O4*D13</f>
         <v>45</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
         <v>650000</v>
       </c>
@@ -1632,7 +1544,7 @@
         <f>O5*D14</f>
         <v>0.12000000000000002</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f t="shared" si="1"/>
         <v>6000</v>
       </c>
@@ -1655,15 +1567,15 @@
       <c r="I16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="4">
         <f>E2</f>
         <v>1000000</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="4">
         <f>SUM(F11:F14)</f>
         <v>1326000</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="4">
         <f>K16-J16</f>
         <v>326000</v>
       </c>

</xml_diff>